<commit_message>
Cambios de Codigo en la ventana gestion estudiante
</commit_message>
<xml_diff>
--- a/Tareas.xlsx
+++ b/Tareas.xlsx
@@ -313,6 +313,87 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -412,33 +493,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -474,15 +528,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -492,51 +537,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -820,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E4:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21:K25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,293 +838,293 @@
   <sheetData>
     <row r="4" spans="5:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="5:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="72" t="s">
+      <c r="F5" s="70"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="73"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="75"/>
-      <c r="M5" s="72" t="s">
+      <c r="J5" s="37"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="73"/>
-      <c r="O5" s="74"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="38"/>
     </row>
     <row r="6" spans="5:15" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="66"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="76"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="67"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="76"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="68"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="14"/>
     </row>
     <row r="7" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E7" s="54" t="s">
+      <c r="E7" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="55"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="78"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="80"/>
-      <c r="L7" s="76"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="46"/>
-      <c r="O7" s="47"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="20"/>
     </row>
     <row r="8" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E8" s="57"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="81"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="83"/>
-      <c r="L8" s="76"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="49"/>
-      <c r="O8" s="50"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="23"/>
     </row>
     <row r="9" spans="5:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E9" s="60"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="76"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="52"/>
-      <c r="O9" s="53"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="26"/>
     </row>
     <row r="10" spans="5:15" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="69"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="71"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="76"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="52"/>
-      <c r="O10" s="53"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="26"/>
     </row>
     <row r="11" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E11" s="45"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="76"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="76"/>
-      <c r="M11" s="33" t="s">
+      <c r="E11" s="18"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="N11" s="34"/>
-      <c r="O11" s="35"/>
+      <c r="N11" s="61"/>
+      <c r="O11" s="62"/>
     </row>
     <row r="12" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E12" s="48"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="76"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="76"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="38"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="64"/>
+      <c r="O12" s="65"/>
     </row>
     <row r="13" spans="5:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E13" s="51"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="76"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="76"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="40"/>
-      <c r="O13" s="41"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="68"/>
     </row>
     <row r="14" spans="5:15" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E14" s="66"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="76"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="76"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="53"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="26"/>
     </row>
     <row r="15" spans="5:15" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E15" s="66"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="68"/>
-      <c r="H15" s="76"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="67"/>
-      <c r="K15" s="68"/>
-      <c r="L15" s="76"/>
-      <c r="M15" s="30" t="s">
+      <c r="E15" s="12"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="N15" s="31"/>
-      <c r="O15" s="32"/>
+      <c r="N15" s="58"/>
+      <c r="O15" s="59"/>
     </row>
     <row r="16" spans="5:15" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="63"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="76"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="76"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="52"/>
-      <c r="O16" s="53"/>
+      <c r="E16" s="81"/>
+      <c r="F16" s="82"/>
+      <c r="G16" s="83"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="26"/>
     </row>
     <row r="17" spans="5:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="18"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="22"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="76"/>
-      <c r="I17" s="78"/>
-      <c r="J17" s="79"/>
-      <c r="K17" s="80"/>
-      <c r="L17" s="76"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="47"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="50"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="20"/>
     </row>
     <row r="18" spans="5:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E18" s="24"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="76"/>
-      <c r="I18" s="81"/>
-      <c r="J18" s="82"/>
-      <c r="K18" s="83"/>
-      <c r="L18" s="76"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="49"/>
-      <c r="O18" s="50"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="23"/>
     </row>
     <row r="19" spans="5:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="27"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="76"/>
-      <c r="I19" s="84"/>
-      <c r="J19" s="85"/>
-      <c r="K19" s="86"/>
-      <c r="L19" s="76"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="52"/>
-      <c r="O19" s="53"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="55"/>
+      <c r="K19" s="56"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="26"/>
     </row>
     <row r="20" spans="5:15" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E20" s="9"/>
       <c r="F20" s="10"/>
       <c r="G20" s="11"/>
-      <c r="H20" s="76"/>
+      <c r="H20" s="16"/>
       <c r="I20" s="3"/>
       <c r="J20" s="4"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="76"/>
+      <c r="L20" s="16"/>
       <c r="M20" s="6"/>
       <c r="N20" s="7"/>
       <c r="O20" s="8"/>
     </row>
     <row r="21" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="76"/>
-      <c r="I21" s="78"/>
-      <c r="J21" s="79"/>
-      <c r="K21" s="80"/>
-      <c r="L21" s="76"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="46"/>
-      <c r="O21" s="47"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="20"/>
     </row>
     <row r="22" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E22" s="15"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="76"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="82"/>
-      <c r="K22" s="83"/>
-      <c r="L22" s="76"/>
-      <c r="M22" s="48"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="50"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="23"/>
     </row>
     <row r="23" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E23" s="15"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="76"/>
-      <c r="I23" s="81"/>
-      <c r="J23" s="82"/>
-      <c r="K23" s="83"/>
-      <c r="L23" s="76"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="49"/>
-      <c r="O23" s="50"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="23"/>
     </row>
     <row r="24" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E24" s="15"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="76"/>
-      <c r="I24" s="81"/>
-      <c r="J24" s="82"/>
-      <c r="K24" s="83"/>
-      <c r="L24" s="76"/>
-      <c r="M24" s="48"/>
-      <c r="N24" s="49"/>
-      <c r="O24" s="50"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="23"/>
     </row>
     <row r="25" spans="5:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="18"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="84"/>
-      <c r="J25" s="85"/>
-      <c r="K25" s="86"/>
-      <c r="L25" s="77"/>
-      <c r="M25" s="51"/>
-      <c r="N25" s="52"/>
-      <c r="O25" s="53"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="26"/>
     </row>
     <row r="26" spans="5:15" x14ac:dyDescent="0.25">
       <c r="H26" s="2"/>
@@ -1158,24 +1158,9 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="H5:H25"/>
-    <mergeCell ref="L5:L25"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="M21:O25"/>
-    <mergeCell ref="M17:O19"/>
-    <mergeCell ref="M7:O9"/>
-    <mergeCell ref="I21:K25"/>
+    <mergeCell ref="E17:G19"/>
+    <mergeCell ref="E21:G25"/>
     <mergeCell ref="I17:K19"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I11:K13"/>
-    <mergeCell ref="I7:K9"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="E21:G25"/>
-    <mergeCell ref="E17:G19"/>
     <mergeCell ref="M15:O15"/>
     <mergeCell ref="M11:O13"/>
     <mergeCell ref="E5:G5"/>
@@ -1190,6 +1175,21 @@
     <mergeCell ref="I16:K16"/>
     <mergeCell ref="I14:K14"/>
     <mergeCell ref="I10:K10"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="H5:H25"/>
+    <mergeCell ref="L5:L25"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M21:O25"/>
+    <mergeCell ref="M17:O19"/>
+    <mergeCell ref="M7:O9"/>
+    <mergeCell ref="I21:K25"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I11:K13"/>
+    <mergeCell ref="I7:K9"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="M14:O14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>